<commit_message>
new routes added, tables added to bd script
</commit_message>
<xml_diff>
--- a/NouvellesAdressesAPI.xlsx
+++ b/NouvellesAdressesAPI.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavobertoldi/Projects/CortevaApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8BADC4F-4AE9-2642-A392-123096E92EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B9A454-B8B5-2B4E-98B6-1EA292DF8F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{54FAB11A-8D98-1647-931E-C44575CDB9D0}"/>
+    <workbookView xWindow="1080" yWindow="1820" windowWidth="28040" windowHeight="17440" xr2:uid="{54FAB11A-8D98-1647-931E-C44575CDB9D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Ancien</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Route::get('users/{username}', FormController::class.'@get');</t>
+  </si>
+  <si>
+    <t>Route::get('machines/{productionlineID}', FormController::class.'@getMachines');</t>
+  </si>
+  <si>
+    <t>Route::get('speedLosses/{PO}/{productionLine}', FormController::class.'@get_speedLosses');</t>
+  </si>
+  <si>
+    <t>Route::get('pos/{shift}/{site}', FormController::class.'@getPOsFromShift');</t>
+  </si>
+  <si>
+    <t>Route::get('events/{PO}/{productionLine}', FormController::class.'@getEvents');</t>
   </si>
 </sst>
 </file>
@@ -426,16 +438,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD05C86A-2F67-E548-8C08-7F64B2A36E8D}">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" customWidth="1"/>
-    <col min="2" max="2" width="38.83203125" customWidth="1"/>
+    <col min="1" max="1" width="83" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -472,6 +484,42 @@
         <v>localhost:5000/api/users/{username}</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <f>_xlfn.CONCAT($B$2,"machine/{producitonLineId}")</f>
+        <v>localhost:5000/api/machine/{producitonLineId}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <f>_xlfn.CONCAT($B$2,"speedloss/{po}/{productionLine}")</f>
+        <v>localhost:5000/api/speedloss/{po}/{productionLine}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <f>_xlfn.CONCAT($B$2,"pos/{shift}/{site}")</f>
+        <v>localhost:5000/api/pos/{shift}/{site}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <f>_xlfn.CONCAT($B$2,"events/{po}/{productionline}")</f>
+        <v>localhost:5000/api/events/{po}/{productionline}</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
All get routes added
</commit_message>
<xml_diff>
--- a/NouvellesAdressesAPI.xlsx
+++ b/NouvellesAdressesAPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavobertoldi/Projects/CortevaApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E5680B-C50D-F648-8B54-F5897FE73695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98786607-D136-F248-A4C7-972962EBACA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="1280" windowWidth="28040" windowHeight="17440" xr2:uid="{54FAB11A-8D98-1647-931E-C44575CDB9D0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Ancien</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Route::get('netOP/{GMID}', FormController::class.'@getNetOP');</t>
+  </si>
+  <si>
+    <t>Route::get('getSpeedLosses/{site}/{productionLine}/{beginningDate}/{endingDate}', FormController::class.'@getSpeedLosses');</t>
+  </si>
+  <si>
+    <t>Route::get('performance/{PO}', FormController::class.'@getPerformanceForASite');</t>
   </si>
 </sst>
 </file>
@@ -468,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD05C86A-2F67-E548-8C08-7F64B2A36E8D}">
-  <dimension ref="A2:B21"/>
+  <dimension ref="A2:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
@@ -528,8 +534,8 @@
         <v>7</v>
       </c>
       <c r="B9" t="str">
-        <f>_xlfn.CONCAT($B$2,"speedloss/{po}/{productionLine}")</f>
-        <v>localhost:5000/api/speedloss/{po}/{productionLine}</v>
+        <f>_xlfn.CONCAT($B$2,"speedlosses/{po}/{productionLine}")</f>
+        <v>localhost:5000/api/speedlosses/{po}/{productionLine}</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -638,6 +644,24 @@
       <c r="B21" t="str">
         <f>_xlfn.CONCAT($B$2,"netOP/{GMID}")</f>
         <v>localhost:5000/api/netOP/{GMID}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <f>_xlfn.CONCAT($B$2,"performance/{PO}")</f>
+        <v>localhost:5000/api/performance/{PO}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="str">
+        <f>_xlfn.CONCAT($B$2,"getSpeedLosses/{site}/{productionLine}/{startingDate}/{endingDate}")</f>
+        <v>localhost:5000/api/getSpeedLosses/{site}/{productionLine}/{startingDate}/{endingDate}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>